<commit_message>
added details on data structure
</commit_message>
<xml_diff>
--- a/inst/extdata/Ind1.xlsx
+++ b/inst/extdata/Ind1.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenajovic/Desktop/BCB410 - R/PerfOMICS/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C44171-AF31-8643-A0A9-58CD657F2593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBA6ECF-09EC-A04C-A075-173213D24C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26000" yWindow="-20440" windowWidth="19700" windowHeight="15460" xr2:uid="{743F6307-FA8E-2040-8484-2209CADB409E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -107,12 +107,6 @@
     <t>10.5/10.5kb</t>
   </si>
   <si>
-    <t>9+9</t>
-  </si>
-  <si>
-    <t>985+185/117/0</t>
-  </si>
-  <si>
     <t>GG</t>
   </si>
   <si>
@@ -174,6 +168,12 @@
   </si>
   <si>
     <t>XX</t>
+  </si>
+  <si>
+    <t>+9+9</t>
+  </si>
+  <si>
+    <t>985+185/1170</t>
   </si>
 </sst>
 </file>
@@ -266,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -284,6 +284,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -601,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0AB25D4-D12E-6840-813A-46C0A40B13CC}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="139" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -613,10 +616,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -632,7 +635,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -656,7 +659,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -669,7 +672,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>21</v>
@@ -677,7 +680,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>22</v>
@@ -687,8 +690,8 @@
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>23</v>
+      <c r="B10" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -696,23 +699,23 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -720,7 +723,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -736,31 +739,31 @@
         <v>10</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -768,7 +771,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -776,7 +779,7 @@
         <v>12</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -784,7 +787,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -792,7 +795,7 @@
         <v>14</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -800,7 +803,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>